<commit_message>
Add references and more
</commit_message>
<xml_diff>
--- a/table2.xlsx
+++ b/table2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/roberto/Desktop/THESIS/HRS/git/icmla_poster/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reisanar/Google Drive/FL_Poly/research_and_other_publications/icmla_poster/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53FF3C26-9407-9444-A74C-EC8292FD4332}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93462C01-51F3-9447-B92B-B781FFF42E09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="860" yWindow="1000" windowWidth="24660" windowHeight="15000" xr2:uid="{30D2AD4B-129E-0D48-BB5E-9FD1D88368CB}"/>
   </bookViews>
@@ -55,15 +55,6 @@
     <t>Category</t>
   </si>
   <si>
-    <t xml:space="preserve">	nk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	fk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	Ctrk</t>
-  </si>
-  <si>
     <t>sophisticated	Not	at	all</t>
   </si>
   <si>
@@ -191,6 +182,15 @@
   </si>
   <si>
     <t xml:space="preserve">	0.01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	$\text{Ctr}_k$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	$f_k$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	$n_k$</t>
   </si>
 </sst>
 </file>
@@ -550,7 +550,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -565,181 +565,181 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>45</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>